<commit_message>
add status excel file for all counties
</commit_message>
<xml_diff>
--- a/County-SO-Data/Status.xlsx
+++ b/County-SO-Data/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\wa-pursuit-pdr-data\County-SO-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3295FCF4-B4FE-4411-AA28-6070726A94EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBF45C6-A11B-4F6C-B392-FA7B91BA42C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{56BC7040-80D7-46AF-88EF-26FB394D08A0}"/>
   </bookViews>
@@ -435,12 +435,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -449,6 +443,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,39 +786,39 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="58.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -826,7 +826,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -834,7 +834,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -842,7 +842,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -850,29 +850,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -880,7 +880,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -888,18 +888,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -907,7 +907,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -915,7 +915,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -923,7 +923,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -931,18 +931,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -950,7 +950,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -958,7 +958,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -966,7 +966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -974,18 +974,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -993,18 +993,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1020,29 +1020,29 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1050,18 +1050,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1077,18 +1077,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1096,18 +1096,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1115,29 +1115,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -1145,18 +1145,18 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -1185,216 +1185,216 @@
       <selection activeCell="A39" sqref="A1:A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+    <col min="1" max="1" width="46.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="8"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
+    <row r="42" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>